<commit_message>
Changed the output name in XLSX files for MainStemPopulation
</commit_message>
<xml_diff>
--- a/Tests/Validation/Barley/Observations/ABlock99_00_BiomassEar.xlsx
+++ b/Tests/Validation/Barley/Observations/ABlock99_00_BiomassEar.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\ApsimX\Prototypes\Barley\Observations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ApsimX\Tests\Validation\Barley\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F017AFF-F118-41DA-90E1-04724AF55F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="20805"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +37,6 @@
   </si>
   <si>
     <t>Barley.Ear.Wt</t>
-  </si>
-  <si>
-    <t>Barley.Structure.MainStemPopn</t>
   </si>
   <si>
     <t>ABlock99_00SowMayPop100</t>
@@ -88,11 +86,14 @@
   <si>
     <t>ABlock99_00SowNovPop500</t>
   </si>
+  <si>
+    <t>Barley.Leaf.MainStemPopulation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -407,20 +408,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,12 +435,12 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>36466</v>
@@ -454,9 +455,9 @@
         <v>692.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>36472</v>
@@ -471,9 +472,9 @@
         <v>777.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>36479</v>
@@ -488,9 +489,9 @@
         <v>777.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>36486</v>
@@ -502,12 +503,12 @@
         <v>557.54947843903869</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>36493</v>
@@ -519,12 +520,12 @@
         <v>533.76014305326521</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>36500</v>
@@ -536,12 +537,12 @@
         <v>896.99839035427476</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>36507</v>
@@ -553,29 +554,29 @@
         <v>837.60158290909408</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>36517</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
         <v>36546</v>
@@ -587,12 +588,12 @@
         <v>1051.911480567667</v>
       </c>
       <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>36462</v>
@@ -607,9 +608,9 @@
         <v>841.25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
         <v>36472</v>
@@ -624,9 +625,9 @@
         <v>921.25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>36479</v>
@@ -641,9 +642,9 @@
         <v>921.25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1">
         <v>36486</v>
@@ -655,12 +656,12 @@
         <v>621.72555168344024</v>
       </c>
       <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
       </c>
       <c r="B15" s="1">
         <v>36493</v>
@@ -672,12 +673,12 @@
         <v>829.80758539094074</v>
       </c>
       <c r="E15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
       </c>
       <c r="B16" s="1">
         <v>36500</v>
@@ -689,12 +690,12 @@
         <v>1057.3194421478211</v>
       </c>
       <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>7</v>
       </c>
       <c r="B17" s="1">
         <v>36507</v>
@@ -706,29 +707,29 @@
         <v>1145.5291505278924</v>
       </c>
       <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
       </c>
       <c r="B18" s="1">
         <v>36517</v>
       </c>
       <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
       </c>
       <c r="B19" s="1">
         <v>36546</v>
@@ -740,12 +741,12 @@
         <v>1104.6161799980816</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1">
         <v>36455</v>
@@ -760,9 +761,9 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1">
         <v>36459</v>
@@ -777,9 +778,9 @@
         <v>997.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1">
         <v>36472</v>
@@ -794,9 +795,9 @@
         <v>1067.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1">
         <v>36479</v>
@@ -811,9 +812,9 @@
         <v>1067.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1">
         <v>36486</v>
@@ -825,12 +826,12 @@
         <v>834.03098411502799</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="1">
         <v>36493</v>
@@ -842,12 +843,12 @@
         <v>946.03792872376073</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1">
         <v>36500</v>
@@ -859,12 +860,12 @@
         <v>1008.4505782800754</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1">
         <v>36507</v>
@@ -876,29 +877,29 @@
         <v>1142.1846974741961</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1">
         <v>36517</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1">
         <v>36546</v>
@@ -910,12 +911,12 @@
         <v>1006.1296883249206</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="1">
         <v>36455</v>
@@ -930,9 +931,9 @@
         <v>1063.3333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="1">
         <v>36459</v>
@@ -947,9 +948,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="1">
         <v>36472</v>
@@ -964,9 +965,9 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="1">
         <v>36479</v>
@@ -981,9 +982,9 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" s="1">
         <v>36486</v>
@@ -995,12 +996,12 @@
         <v>883.40873994722278</v>
       </c>
       <c r="E34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="1">
         <v>36493</v>
@@ -1012,12 +1013,12 @@
         <v>978.74190372848136</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="1">
         <v>36500</v>
@@ -1029,12 +1030,12 @@
         <v>1043.7757095819754</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" s="1">
         <v>36507</v>
@@ -1046,29 +1047,29 @@
         <v>1120.7478346135624</v>
       </c>
       <c r="E37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1">
         <v>36517</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="1">
         <v>36546</v>
@@ -1080,12 +1081,12 @@
         <v>989.09776910938945</v>
       </c>
       <c r="E39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="1">
         <v>36472</v>
@@ -1100,9 +1101,9 @@
         <v>788.75</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" s="1">
         <v>36479</v>
@@ -1117,9 +1118,9 @@
         <v>788.75</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" s="1">
         <v>36486</v>
@@ -1131,12 +1132,12 @@
         <v>696.16872274971081</v>
       </c>
       <c r="E42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" s="1">
         <v>36493</v>
@@ -1148,12 +1149,12 @@
         <v>703.35109067584631</v>
       </c>
       <c r="E43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" s="1">
         <v>36500</v>
@@ -1165,12 +1166,12 @@
         <v>925.8499138129871</v>
       </c>
       <c r="E44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" s="1">
         <v>36507</v>
@@ -1182,29 +1183,29 @@
         <v>1253.2594188492515</v>
       </c>
       <c r="E45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="1">
         <v>36517</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="1">
         <v>36546</v>
@@ -1216,12 +1217,12 @@
         <v>1067.3014489238817</v>
       </c>
       <c r="E47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" s="1">
         <v>36493</v>
@@ -1233,12 +1234,12 @@
         <v>132.86791385095705</v>
       </c>
       <c r="E48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="1">
         <v>36500</v>
@@ -1250,12 +1251,12 @@
         <v>160.74203746830625</v>
       </c>
       <c r="E49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="1">
         <v>36507</v>
@@ -1267,12 +1268,12 @@
         <v>421.47068409115417</v>
       </c>
       <c r="E50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" s="1">
         <v>36517</v>
@@ -1284,12 +1285,12 @@
         <v>541.56820765987584</v>
       </c>
       <c r="E51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" s="1">
         <v>36535</v>
@@ -1301,12 +1302,12 @@
         <v>1042.4657669061723</v>
       </c>
       <c r="E52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" s="1">
         <v>36542</v>
@@ -1318,29 +1319,29 @@
         <v>1202.6650320327899</v>
       </c>
       <c r="E53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="1">
         <v>36550</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" s="1">
         <v>36564</v>
@@ -1352,12 +1353,12 @@
         <v>1108.1506998976208</v>
       </c>
       <c r="E55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1">
         <v>36524</v>
@@ -1369,12 +1370,12 @@
         <v>827.38384048265152</v>
       </c>
       <c r="E56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" s="1">
         <v>36488</v>
@@ -1386,12 +1387,12 @@
         <v>158.11535388623537</v>
       </c>
       <c r="E57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58" s="1">
         <v>36490</v>
@@ -1403,12 +1404,12 @@
         <v>154.76196923116802</v>
       </c>
       <c r="E58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59" s="1">
         <v>36493</v>
@@ -1420,12 +1421,12 @@
         <v>174.64679341292779</v>
       </c>
       <c r="E59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B60" s="1">
         <v>36500</v>
@@ -1437,12 +1438,12 @@
         <v>217.43971452390679</v>
       </c>
       <c r="E60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B61" s="1">
         <v>36507</v>
@@ -1454,12 +1455,12 @@
         <v>460.90887700043368</v>
       </c>
       <c r="E61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B62" s="1">
         <v>36517</v>
@@ -1471,12 +1472,12 @@
         <v>697.94876976271496</v>
       </c>
       <c r="E62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" s="1">
         <v>36535</v>
@@ -1488,12 +1489,12 @@
         <v>1045.840665639897</v>
       </c>
       <c r="E63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B64" s="1">
         <v>36542</v>
@@ -1505,29 +1506,29 @@
         <v>1125.3747353706822</v>
       </c>
       <c r="E64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B65" s="1">
         <v>36550</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B66" s="1">
         <v>36564</v>
@@ -1539,12 +1540,12 @@
         <v>1022.5441697218268</v>
       </c>
       <c r="E66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B67" s="1">
         <v>36524</v>
@@ -1556,12 +1557,12 @@
         <v>948.09714962673013</v>
       </c>
       <c r="E67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B68" s="1">
         <v>36488</v>
@@ -1573,12 +1574,12 @@
         <v>136.06216814934683</v>
       </c>
       <c r="E68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B69" s="1">
         <v>36493</v>
@@ -1590,12 +1591,12 @@
         <v>185.28079205951508</v>
       </c>
       <c r="E69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B70" s="1">
         <v>36500</v>
@@ -1607,12 +1608,12 @@
         <v>226.83822634582302</v>
       </c>
       <c r="E70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B71" s="1">
         <v>36507</v>
@@ -1624,12 +1625,12 @@
         <v>494.7965107240359</v>
       </c>
       <c r="E71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B72" s="1">
         <v>36517</v>
@@ -1641,12 +1642,12 @@
         <v>799.51193890509694</v>
       </c>
       <c r="E72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B73" s="1">
         <v>36535</v>
@@ -1658,12 +1659,12 @@
         <v>1140.7011606259221</v>
       </c>
       <c r="E73" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B74" s="1">
         <v>36542</v>
@@ -1675,29 +1676,29 @@
         <v>1099.4505803251911</v>
       </c>
       <c r="E74" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B75" s="1">
         <v>36550</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E75" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B76" s="1">
         <v>36564</v>
@@ -1709,12 +1710,12 @@
         <v>1029.1577850164497</v>
       </c>
       <c r="E76" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B77" s="1">
         <v>36524</v>
@@ -1726,12 +1727,12 @@
         <v>858.94250687463727</v>
       </c>
       <c r="E77" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B78" s="1">
         <v>36486</v>
@@ -1743,12 +1744,12 @@
         <v>159.52428282732413</v>
       </c>
       <c r="E78" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B79" s="1">
         <v>36493</v>
@@ -1760,12 +1761,12 @@
         <v>198.05957028711251</v>
       </c>
       <c r="E79" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B80" s="1">
         <v>36500</v>
@@ -1777,12 +1778,12 @@
         <v>339.65179896981584</v>
       </c>
       <c r="E80" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B81" s="1">
         <v>36507</v>
@@ -1794,12 +1795,12 @@
         <v>534.3498537990165</v>
       </c>
       <c r="E81" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B82" s="1">
         <v>36517</v>
@@ -1811,12 +1812,12 @@
         <v>864.19848035813106</v>
       </c>
       <c r="E82" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B83" s="1">
         <v>36535</v>
@@ -1828,12 +1829,12 @@
         <v>1136.5110191538301</v>
       </c>
       <c r="E83" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B84" s="1">
         <v>36542</v>
@@ -1845,29 +1846,29 @@
         <v>1228.2372991899203</v>
       </c>
       <c r="E84" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B85" s="1">
         <v>36550</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B86" s="1">
         <v>36564</v>
@@ -1879,12 +1880,12 @@
         <v>945.47956307281231</v>
       </c>
       <c r="E86" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B87" s="1">
         <v>36524</v>
@@ -1896,12 +1897,12 @@
         <v>1079.8898571770176</v>
       </c>
       <c r="E87" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B88" s="1">
         <v>36493</v>
@@ -1913,12 +1914,12 @@
         <v>151.16478758785121</v>
       </c>
       <c r="E88" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89" s="1">
         <v>36500</v>
@@ -1930,12 +1931,12 @@
         <v>187.28708320033462</v>
       </c>
       <c r="E89" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B90" s="1">
         <v>36507</v>
@@ -1947,12 +1948,12 @@
         <v>416.7330047488831</v>
       </c>
       <c r="E90" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B91" s="1">
         <v>36517</v>
@@ -1964,12 +1965,12 @@
         <v>581.9394618437592</v>
       </c>
       <c r="E91" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B92" s="1">
         <v>36535</v>
@@ -1981,12 +1982,12 @@
         <v>1212.2644855428921</v>
       </c>
       <c r="E92" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B93" s="1">
         <v>36542</v>
@@ -1998,29 +1999,29 @@
         <v>1182.9444501429314</v>
       </c>
       <c r="E93" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B94" s="1">
         <v>36550</v>
       </c>
       <c r="C94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E94" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B95" s="1">
         <v>36564</v>
@@ -2032,12 +2033,12 @@
         <v>1008.3322114577539</v>
       </c>
       <c r="E95" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B96" s="1">
         <v>36524</v>
@@ -2049,12 +2050,12 @@
         <v>856.42577959808432</v>
       </c>
       <c r="E96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B97" s="1">
         <v>36553</v>
@@ -2066,12 +2067,12 @@
         <v>155.39376271883447</v>
       </c>
       <c r="E97" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B98" s="1">
         <v>36556</v>
@@ -2083,12 +2084,12 @@
         <v>204.74024366318056</v>
       </c>
       <c r="E98" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B99" s="1">
         <v>36570</v>
@@ -2100,12 +2101,12 @@
         <v>590.51194495794766</v>
       </c>
       <c r="E99" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B100" s="1">
         <v>36577</v>
@@ -2117,12 +2118,12 @@
         <v>624.21974983994835</v>
       </c>
       <c r="E100" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B101" s="1">
         <v>36584</v>
@@ -2134,29 +2135,29 @@
         <v>839.66867966673919</v>
       </c>
       <c r="E101" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B102" s="1">
         <v>36591</v>
       </c>
       <c r="C102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E102" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B103" s="1">
         <v>36602</v>
@@ -2168,12 +2169,12 @@
         <v>719.0280288407082</v>
       </c>
       <c r="E103" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B104" s="1">
         <v>36550</v>
@@ -2185,12 +2186,12 @@
         <v>167.84149709141104</v>
       </c>
       <c r="E104" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B105" s="1">
         <v>36556</v>
@@ -2202,12 +2203,12 @@
         <v>241.83746870805561</v>
       </c>
       <c r="E105" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B106" s="1">
         <v>36570</v>
@@ -2219,12 +2220,12 @@
         <v>584.07006088788501</v>
       </c>
       <c r="E106" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B107" s="1">
         <v>36577</v>
@@ -2236,12 +2237,12 @@
         <v>746.94617899410423</v>
       </c>
       <c r="E107" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B108" s="1">
         <v>36584</v>
@@ -2253,29 +2254,29 @@
         <v>750.65011509864621</v>
       </c>
       <c r="E108" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B109" s="1">
         <v>36591</v>
       </c>
       <c r="C109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B110" s="1">
         <v>36602</v>
@@ -2287,12 +2288,12 @@
         <v>701.97395675942448</v>
       </c>
       <c r="E110" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B111" s="1">
         <v>36550</v>
@@ -2304,12 +2305,12 @@
         <v>178.33319068066868</v>
       </c>
       <c r="E111" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B112" s="1">
         <v>36556</v>
@@ -2321,12 +2322,12 @@
         <v>279.04304452780769</v>
       </c>
       <c r="E112" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B113" s="1">
         <v>36570</v>
@@ -2338,12 +2339,12 @@
         <v>619.15858471310685</v>
       </c>
       <c r="E113" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B114" s="1">
         <v>36577</v>
@@ -2355,12 +2356,12 @@
         <v>726.03134107905237</v>
       </c>
       <c r="E114" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B115" s="1">
         <v>36584</v>
@@ -2372,29 +2373,29 @@
         <v>728.81833036604974</v>
       </c>
       <c r="E115" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B116" s="1">
         <v>36591</v>
       </c>
       <c r="C116" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E116" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B117" s="1">
         <v>36602</v>
@@ -2406,12 +2407,12 @@
         <v>807.63099485733176</v>
       </c>
       <c r="E117" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B118" s="1">
         <v>36546</v>
@@ -2423,12 +2424,12 @@
         <v>182.3464254610642</v>
       </c>
       <c r="E118" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B119" s="1">
         <v>36556</v>
@@ -2440,12 +2441,12 @@
         <v>334.48447048595341</v>
       </c>
       <c r="E119" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B120" s="1">
         <v>36570</v>
@@ -2457,12 +2458,12 @@
         <v>675.78558766104902</v>
       </c>
       <c r="E120" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B121" s="1">
         <v>36577</v>
@@ -2474,12 +2475,12 @@
         <v>761.88170850178028</v>
       </c>
       <c r="E121" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B122" s="1">
         <v>36584</v>
@@ -2491,29 +2492,29 @@
         <v>828.90935956415672</v>
       </c>
       <c r="E122" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B123" s="1">
         <v>36591</v>
       </c>
       <c r="C123" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D123" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E123" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B124" s="1">
         <v>36602</v>
@@ -2525,12 +2526,12 @@
         <v>765.89745117977191</v>
       </c>
       <c r="E124" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B125" s="1">
         <v>36556</v>
@@ -2542,12 +2543,12 @@
         <v>206.42336512156763</v>
       </c>
       <c r="E125" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B126" s="1">
         <v>36570</v>
@@ -2559,12 +2560,12 @@
         <v>591.46190686872399</v>
       </c>
       <c r="E126" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B127" s="1">
         <v>36577</v>
@@ -2576,12 +2577,12 @@
         <v>746.59970076448701</v>
       </c>
       <c r="E127" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B128" s="1">
         <v>36584</v>
@@ -2593,29 +2594,29 @@
         <v>790.24082965105129</v>
       </c>
       <c r="E128" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B129" s="1">
         <v>36591</v>
       </c>
       <c r="C129" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D129" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E129" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B130" s="1">
         <v>36602</v>
@@ -2627,7 +2628,7 @@
         <v>669.46419821261088</v>
       </c>
       <c r="E130" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>